<commit_message>
Vivalata les modifs !
</commit_message>
<xml_diff>
--- a/données erreurs et seuils.xlsx
+++ b/données erreurs et seuils.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dragonlysa18\Documents\FISE 2\Semestre 8\TD\TD classification bayésienne-20180313\RdF_Exo2_Partie1\RdF_Exo2_Partie1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dragonlysa18\Documents\FISE 2\Semestre 8\Reconnaissance de forme\TD Bayésien\TD classification bayésienne-20180313\TD_github\TD-a-rendre-Reconnaissances-de-formes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{035AB607-B366-4256-9A76-357EE330F7AB}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E181A8-1287-47AC-9DA8-3EB9CE38139A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{52A36B64-12EF-437F-A86D-249273682ED4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>Perreur</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>xb</t>
+  </si>
+  <si>
+    <t>xb2</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -63,7 +69,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -71,13 +77,116 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,92 +501,165 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8052BC88-5467-4D81-AB0D-8663D4292371}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="E1" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>0.5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>0.36180000000000001</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>7.8700000000000006E-2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="E3" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5">
+        <f xml:space="preserve"> (32 + J5)/2*15</f>
+        <v>291.17401789029697</v>
+      </c>
+      <c r="E4" s="6">
+        <f xml:space="preserve"> (32 - J5)/2*15</f>
+        <v>188.82598210970303</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>1</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5">
+        <f xml:space="preserve"> (-1 + K5)</f>
+        <v>0.64108110115251327</v>
+      </c>
+      <c r="E5" s="6">
+        <f xml:space="preserve"> (-1 - K5)</f>
+        <v>-2.6410811011525133</v>
+      </c>
+      <c r="J5">
+        <f>SQRT(J6)</f>
+        <v>6.8232023853729293</v>
+      </c>
+      <c r="K5">
+        <f>SQRT(K6)</f>
+        <v>1.6410811011525133</v>
+      </c>
+      <c r="L5">
+        <f>SQRT(L6)</f>
+        <v>10.470553195639372</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>1</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5">
+        <f>(-2+2*L5)/14</f>
+        <v>1.3529361708056247</v>
+      </c>
+      <c r="E6" s="5">
+        <f>(-2-2*L5)/14</f>
+        <v>-1.6386504565199103</v>
+      </c>
+      <c r="J6">
+        <f>256-4*7*(8-3/4*LN(2))</f>
+        <v>46.556090791758834</v>
+      </c>
+      <c r="K6">
+        <f>2+LN(2)</f>
+        <v>2.6931471805599454</v>
+      </c>
+      <c r="L6">
+        <f>4+4*7*(1+4*LN(2))</f>
+        <v>109.63248422271387</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="8">
         <v>0.23980000000000001</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="9">
         <v>0.5</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <f>LN(2)</f>
+        <v>0.69314718055994529</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <f>SQRT(3)</f>
+        <v>1.7320508075688772</v>
       </c>
     </row>
   </sheetData>

</xml_diff>